<commit_message>
fix container test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/intakemanifest_holding_w_child_template.xlsx
+++ b/src/test/resources/intakemanifest_holding_w_child_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgonzales/IdeaProjects/testing/cora/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpatel/eclipse-workspace/cora/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27184D28-B19E-954C-A967-FC36587FD3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EBC45CE-7DCE-C74D-88D1-7D345075BCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="210">
   <si>
     <t>Cora INTAKE manifest</t>
   </si>
@@ -680,6 +680,12 @@
   </si>
   <si>
     <t>afddf</t>
+  </si>
+  <si>
+    <t>Project.Var11</t>
+  </si>
+  <si>
+    <t>Project.Var12</t>
   </si>
 </sst>
 </file>
@@ -1466,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE43"/>
+  <dimension ref="A1:BF43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BF5" sqref="BF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1508,10 +1514,10 @@
     <col min="45" max="45" width="36.83203125" style="22" customWidth="1"/>
     <col min="46" max="46" width="20" style="22" customWidth="1"/>
     <col min="47" max="56" width="15.83203125" style="22" customWidth="1"/>
-    <col min="57" max="57" width="2" customWidth="1"/>
+    <col min="57" max="57" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1569,10 +1575,10 @@
       <c r="BA1" s="17"/>
       <c r="BB1" s="17"/>
       <c r="BC1" s="17"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="10"/>
-    </row>
-    <row r="2" spans="1:57" ht="26" x14ac:dyDescent="0.2">
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+    </row>
+    <row r="2" spans="1:58" ht="26" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>148</v>
       </c>
@@ -1669,9 +1675,10 @@
       <c r="BB2" s="54"/>
       <c r="BC2" s="54"/>
       <c r="BD2" s="54"/>
-      <c r="BE2" s="10"/>
-    </row>
-    <row r="3" spans="1:57" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE2" s="54"/>
+      <c r="BF2" s="54"/>
+    </row>
+    <row r="3" spans="1:58" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1738,9 +1745,10 @@
       <c r="BB3" s="42"/>
       <c r="BC3" s="42"/>
       <c r="BD3" s="42"/>
-      <c r="BE3" s="10"/>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE3" s="42"/>
+      <c r="BF3" s="42"/>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="45" t="s">
         <v>2</v>
@@ -1907,9 +1915,14 @@
       <c r="BD4" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="BE4" s="10"/>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE4" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="BF4" s="47" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1968,9 +1981,10 @@
       <c r="BB5" s="40"/>
       <c r="BC5" s="40"/>
       <c r="BD5" s="40"/>
-      <c r="BE5" s="10"/>
-    </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE5" s="40"/>
+      <c r="BF5" s="40"/>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -2029,9 +2043,10 @@
       <c r="BB6" s="40"/>
       <c r="BC6" s="40"/>
       <c r="BD6" s="40"/>
-      <c r="BE6" s="10"/>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE6" s="40"/>
+      <c r="BF6" s="40"/>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="12" t="s">
         <v>29</v>
@@ -2106,9 +2121,10 @@
       <c r="BB7" s="28"/>
       <c r="BC7" s="28"/>
       <c r="BD7" s="28"/>
-      <c r="BE7" s="10"/>
-    </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE7" s="28"/>
+      <c r="BF7" s="28"/>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="12" t="s">
         <v>29</v>
@@ -2183,9 +2199,10 @@
       <c r="BB8" s="28"/>
       <c r="BC8" s="28"/>
       <c r="BD8" s="28"/>
-      <c r="BE8" s="10"/>
-    </row>
-    <row r="9" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE8" s="28"/>
+      <c r="BF8" s="28"/>
+    </row>
+    <row r="9" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="12" t="s">
         <v>112</v>
@@ -2268,9 +2285,10 @@
       <c r="BB9" s="28"/>
       <c r="BC9" s="28"/>
       <c r="BD9" s="28"/>
-      <c r="BE9" s="10"/>
-    </row>
-    <row r="10" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE9" s="28"/>
+      <c r="BF9" s="28"/>
+    </row>
+    <row r="10" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="12" t="s">
         <v>112</v>
@@ -2353,9 +2371,10 @@
       <c r="BB10" s="28"/>
       <c r="BC10" s="28"/>
       <c r="BD10" s="28"/>
-      <c r="BE10" s="10"/>
-    </row>
-    <row r="11" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE10" s="28"/>
+      <c r="BF10" s="28"/>
+    </row>
+    <row r="11" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="12" t="s">
         <v>72</v>
@@ -2438,9 +2457,10 @@
       <c r="BB11" s="28"/>
       <c r="BC11" s="28"/>
       <c r="BD11" s="28"/>
-      <c r="BE11" s="10"/>
-    </row>
-    <row r="12" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE11" s="28"/>
+      <c r="BF11" s="28"/>
+    </row>
+    <row r="12" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="12" t="s">
         <v>72</v>
@@ -2523,9 +2543,10 @@
       <c r="BB12" s="28"/>
       <c r="BC12" s="28"/>
       <c r="BD12" s="28"/>
-      <c r="BE12" s="10"/>
-    </row>
-    <row r="13" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE12" s="28"/>
+      <c r="BF12" s="28"/>
+    </row>
+    <row r="13" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="12" t="s">
         <v>73</v>
@@ -2608,9 +2629,10 @@
       <c r="BB13" s="28"/>
       <c r="BC13" s="28"/>
       <c r="BD13" s="28"/>
-      <c r="BE13" s="10"/>
-    </row>
-    <row r="14" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE13" s="28"/>
+      <c r="BF13" s="28"/>
+    </row>
+    <row r="14" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="12" t="s">
         <v>73</v>
@@ -2693,9 +2715,10 @@
       <c r="BB14" s="28"/>
       <c r="BC14" s="28"/>
       <c r="BD14" s="28"/>
-      <c r="BE14" s="10"/>
-    </row>
-    <row r="15" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE14" s="28"/>
+      <c r="BF14" s="28"/>
+    </row>
+    <row r="15" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="12" t="s">
         <v>74</v>
@@ -2778,9 +2801,10 @@
       <c r="BB15" s="28"/>
       <c r="BC15" s="28"/>
       <c r="BD15" s="28"/>
-      <c r="BE15" s="10"/>
-    </row>
-    <row r="16" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE15" s="28"/>
+      <c r="BF15" s="28"/>
+    </row>
+    <row r="16" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="12" t="s">
         <v>74</v>
@@ -2863,9 +2887,10 @@
       <c r="BB16" s="28"/>
       <c r="BC16" s="28"/>
       <c r="BD16" s="28"/>
-      <c r="BE16" s="10"/>
-    </row>
-    <row r="17" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE16" s="28"/>
+      <c r="BF16" s="28"/>
+    </row>
+    <row r="17" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="12" t="s">
         <v>119</v>
@@ -2948,9 +2973,10 @@
       <c r="BB17" s="28"/>
       <c r="BC17" s="28"/>
       <c r="BD17" s="28"/>
-      <c r="BE17" s="10"/>
-    </row>
-    <row r="18" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE17" s="28"/>
+      <c r="BF17" s="28"/>
+    </row>
+    <row r="18" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="12" t="s">
         <v>119</v>
@@ -3033,9 +3059,10 @@
       <c r="BB18" s="28"/>
       <c r="BC18" s="28"/>
       <c r="BD18" s="28"/>
-      <c r="BE18" s="10"/>
-    </row>
-    <row r="19" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE18" s="28"/>
+      <c r="BF18" s="28"/>
+    </row>
+    <row r="19" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="12" t="s">
         <v>113</v>
@@ -3116,9 +3143,10 @@
       <c r="BB19" s="28"/>
       <c r="BC19" s="28"/>
       <c r="BD19" s="28"/>
-      <c r="BE19" s="10"/>
-    </row>
-    <row r="20" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE19" s="28"/>
+      <c r="BF19" s="28"/>
+    </row>
+    <row r="20" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="12" t="s">
         <v>113</v>
@@ -3199,9 +3227,10 @@
       <c r="BB20" s="28"/>
       <c r="BC20" s="28"/>
       <c r="BD20" s="28"/>
-      <c r="BE20" s="10"/>
-    </row>
-    <row r="21" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE20" s="28"/>
+      <c r="BF20" s="28"/>
+    </row>
+    <row r="21" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="12" t="s">
         <v>115</v>
@@ -3284,9 +3313,10 @@
       <c r="BB21" s="28"/>
       <c r="BC21" s="28"/>
       <c r="BD21" s="28"/>
-      <c r="BE21" s="10"/>
-    </row>
-    <row r="22" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE21" s="28"/>
+      <c r="BF21" s="28"/>
+    </row>
+    <row r="22" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="12" t="s">
         <v>115</v>
@@ -3369,9 +3399,10 @@
       <c r="BB22" s="28"/>
       <c r="BC22" s="28"/>
       <c r="BD22" s="28"/>
-      <c r="BE22" s="10"/>
-    </row>
-    <row r="23" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE22" s="28"/>
+      <c r="BF22" s="28"/>
+    </row>
+    <row r="23" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="12" t="s">
         <v>117</v>
@@ -3454,9 +3485,10 @@
       <c r="BB23" s="28"/>
       <c r="BC23" s="28"/>
       <c r="BD23" s="28"/>
-      <c r="BE23" s="10"/>
-    </row>
-    <row r="24" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE23" s="28"/>
+      <c r="BF23" s="28"/>
+    </row>
+    <row r="24" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="12" t="s">
         <v>117</v>
@@ -3539,9 +3571,10 @@
       <c r="BB24" s="28"/>
       <c r="BC24" s="28"/>
       <c r="BD24" s="28"/>
-      <c r="BE24" s="10"/>
-    </row>
-    <row r="25" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE24" s="28"/>
+      <c r="BF24" s="28"/>
+    </row>
+    <row r="25" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="12" t="s">
         <v>89</v>
@@ -3622,9 +3655,10 @@
       <c r="BB25" s="28"/>
       <c r="BC25" s="28"/>
       <c r="BD25" s="28"/>
-      <c r="BE25" s="10"/>
-    </row>
-    <row r="26" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE25" s="28"/>
+      <c r="BF25" s="28"/>
+    </row>
+    <row r="26" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="12" t="s">
         <v>89</v>
@@ -3705,9 +3739,10 @@
       <c r="BB26" s="28"/>
       <c r="BC26" s="28"/>
       <c r="BD26" s="28"/>
-      <c r="BE26" s="10"/>
-    </row>
-    <row r="27" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE26" s="28"/>
+      <c r="BF26" s="28"/>
+    </row>
+    <row r="27" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="12" t="s">
         <v>75</v>
@@ -3788,9 +3823,10 @@
       <c r="BB27" s="28"/>
       <c r="BC27" s="28"/>
       <c r="BD27" s="28"/>
-      <c r="BE27" s="10"/>
-    </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE27" s="28"/>
+      <c r="BF27" s="28"/>
+    </row>
+    <row r="28" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="12" t="s">
         <v>75</v>
@@ -3871,9 +3907,10 @@
       <c r="BB28" s="28"/>
       <c r="BC28" s="28"/>
       <c r="BD28" s="28"/>
-      <c r="BE28" s="10"/>
-    </row>
-    <row r="29" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE28" s="28"/>
+      <c r="BF28" s="28"/>
+    </row>
+    <row r="29" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="12" t="s">
         <v>114</v>
@@ -3954,9 +3991,10 @@
       <c r="BB29" s="28"/>
       <c r="BC29" s="28"/>
       <c r="BD29" s="28"/>
-      <c r="BE29" s="10"/>
-    </row>
-    <row r="30" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE29" s="28"/>
+      <c r="BF29" s="28"/>
+    </row>
+    <row r="30" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="12" t="s">
         <v>114</v>
@@ -4037,9 +4075,10 @@
       <c r="BB30" s="28"/>
       <c r="BC30" s="28"/>
       <c r="BD30" s="28"/>
-      <c r="BE30" s="10"/>
-    </row>
-    <row r="31" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE30" s="28"/>
+      <c r="BF30" s="28"/>
+    </row>
+    <row r="31" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="12" t="s">
         <v>116</v>
@@ -4122,9 +4161,10 @@
       <c r="BB31" s="28"/>
       <c r="BC31" s="28"/>
       <c r="BD31" s="28"/>
-      <c r="BE31" s="10"/>
-    </row>
-    <row r="32" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE31" s="28"/>
+      <c r="BF31" s="28"/>
+    </row>
+    <row r="32" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="12" t="s">
         <v>116</v>
@@ -4207,9 +4247,10 @@
       <c r="BB32" s="28"/>
       <c r="BC32" s="28"/>
       <c r="BD32" s="28"/>
-      <c r="BE32" s="10"/>
-    </row>
-    <row r="33" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE32" s="28"/>
+      <c r="BF32" s="28"/>
+    </row>
+    <row r="33" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="12" t="s">
         <v>118</v>
@@ -4292,9 +4333,10 @@
       <c r="BB33" s="28"/>
       <c r="BC33" s="28"/>
       <c r="BD33" s="28"/>
-      <c r="BE33" s="10"/>
-    </row>
-    <row r="34" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE33" s="28"/>
+      <c r="BF33" s="28"/>
+    </row>
+    <row r="34" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="12" t="s">
         <v>118</v>
@@ -4377,9 +4419,10 @@
       <c r="BB34" s="28"/>
       <c r="BC34" s="28"/>
       <c r="BD34" s="28"/>
-      <c r="BE34" s="10"/>
-    </row>
-    <row r="35" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE34" s="28"/>
+      <c r="BF34" s="28"/>
+    </row>
+    <row r="35" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="12" t="s">
         <v>90</v>
@@ -4460,9 +4503,10 @@
       <c r="BB35" s="28"/>
       <c r="BC35" s="28"/>
       <c r="BD35" s="28"/>
-      <c r="BE35" s="10"/>
-    </row>
-    <row r="36" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE35" s="28"/>
+      <c r="BF35" s="28"/>
+    </row>
+    <row r="36" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="12" t="s">
         <v>90</v>
@@ -4543,9 +4587,10 @@
       <c r="BB36" s="28"/>
       <c r="BC36" s="28"/>
       <c r="BD36" s="28"/>
-      <c r="BE36" s="10"/>
-    </row>
-    <row r="37" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE36" s="28"/>
+      <c r="BF36" s="28"/>
+    </row>
+    <row r="37" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="12" t="s">
         <v>76</v>
@@ -4626,9 +4671,10 @@
       <c r="BB37" s="28"/>
       <c r="BC37" s="28"/>
       <c r="BD37" s="28"/>
-      <c r="BE37" s="10"/>
-    </row>
-    <row r="38" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE37" s="28"/>
+      <c r="BF37" s="28"/>
+    </row>
+    <row r="38" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="12" t="s">
         <v>76</v>
@@ -4709,9 +4755,10 @@
       <c r="BB38" s="28"/>
       <c r="BC38" s="28"/>
       <c r="BD38" s="28"/>
-      <c r="BE38" s="10"/>
-    </row>
-    <row r="39" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE38" s="28"/>
+      <c r="BF38" s="28"/>
+    </row>
+    <row r="39" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="12" t="s">
         <v>200</v>
@@ -4796,9 +4843,10 @@
       <c r="BB39" s="28"/>
       <c r="BC39" s="28"/>
       <c r="BD39" s="28"/>
-      <c r="BE39" s="10"/>
-    </row>
-    <row r="40" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BE39" s="28"/>
+      <c r="BF39" s="28"/>
+    </row>
+    <row r="40" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="12" t="s">
         <v>200</v>
@@ -4883,9 +4931,10 @@
       <c r="BB40" s="28"/>
       <c r="BC40" s="28"/>
       <c r="BD40" s="28"/>
-      <c r="BE40" s="10"/>
-    </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE40" s="28"/>
+      <c r="BF40" s="28"/>
+    </row>
+    <row r="41" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>20</v>
       </c>
@@ -4944,14 +4993,15 @@
       <c r="BB41" s="41"/>
       <c r="BC41" s="41"/>
       <c r="BD41" s="41"/>
-      <c r="BE41" s="10"/>
-    </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BE41" s="41"/>
+      <c r="BF41" s="41"/>
+    </row>
+    <row r="42" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -5405,56 +5455,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009574B466B7C21C4B9D80A860A3E13C1A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd793596002196d52fa40f8a6c8ea08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="87ba4a14-7e41-41c7-9f63-fc9ba18728c1" xmlns:ns3="a134e188-d237-415e-9089-632cc8d2b4a8" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e864093dbf6fe24f04cb571f9b23010" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5681,7 +5681,66 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
@@ -5698,24 +5757,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB796F2-5C91-404E-A982-5BB5583B6419}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030AB9D0-3CD7-41B6-9BD1-2380E994F20B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5736,7 +5778,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DB796F2-5C91-404E-A982-5BB5583B6419}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C995F59-21A4-4074-851C-1BF821ADB8A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FF37FDE-501D-48DC-9178-AA6A40941737}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -5753,12 +5811,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C995F59-21A4-4074-851C-1BF821ADB8A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>